<commit_message>
debug and checkout nest oneToMany
</commit_message>
<xml_diff>
--- a/bookshop.xlsx
+++ b/bookshop.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="0" windowWidth="25600" windowHeight="19820" tabRatio="500"/>
+    <workbookView xWindow="2660" yWindow="0" windowWidth="25600" windowHeight="19820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="category" sheetId="1" r:id="rId1"/>
     <sheet name="book" sheetId="2" r:id="rId2"/>
-    <sheet name="工作表1" sheetId="3" r:id="rId3"/>
-    <sheet name="工作表2" sheetId="4" r:id="rId4"/>
+    <sheet name="pages" sheetId="5" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="3" r:id="rId4"/>
+    <sheet name="工作表2" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -108,10 +109,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>大秦帝国</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>明朝那些事</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -154,6 +151,42 @@
   </si>
   <si>
     <t>oneToMany,bookshop.xlsx,book,category_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pages</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>oneToMany,bookshop.xlsx,pages,book_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>book_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大秦帝国aaaaaa</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>明朝那些bbbbbb事</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ccccc1984</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>万寿寺ddddd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大秦帝国3333</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -161,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,6 +222,24 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,8 +258,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -217,7 +272,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -549,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -607,7 +666,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -626,7 +685,7 @@
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5">
         <f>A5*10</f>
@@ -668,7 +727,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>15</v>
@@ -692,18 +751,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -717,10 +777,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -734,10 +797,13 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -753,8 +819,11 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -762,43 +831,43 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <f>A5*10</f>
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <f>A6*10</f>
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -809,25 +878,25 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <f>A7*10</f>
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8">
         <f>A8*10</f>
@@ -847,6 +916,112 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -864,7 +1039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
remove null key for object
</commit_message>
<xml_diff>
--- a/bookshop.xlsx
+++ b/bookshop.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="0" windowWidth="25600" windowHeight="19820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="36600" yWindow="0" windowWidth="25600" windowHeight="19820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="category" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -220,6 +220,62 @@
   <si>
     <t>eeeeeeee</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>extra_1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>额外 1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>extra_2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>我说哪。</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>hot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>热度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>where</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>位置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>二楼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一楼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -230,7 +286,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -249,7 +305,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -258,7 +314,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -267,7 +323,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -307,13 +363,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -642,10 +698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -654,7 +710,7 @@
     <col min="5" max="5" width="35.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -670,8 +726,14 @@
       <c r="E1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -687,8 +749,14 @@
       <c r="E2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -704,8 +772,14 @@
       <c r="E3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -713,7 +787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75">
+    <row r="5" spans="1:7" ht="75">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -727,8 +801,14 @@
         <f>A5*10</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -743,7 +823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -758,7 +838,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -771,6 +851,12 @@
       <c r="D8">
         <f>A8*10</f>
         <v>40</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -789,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -977,15 +1063,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -995,8 +1081,14 @@
       <c r="C1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1006,8 +1098,11 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1017,8 +1112,14 @@
       <c r="C3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1026,7 +1127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1036,8 +1137,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1048,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1058,8 +1162,11 @@
       <c r="C7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1067,6 +1174,9 @@
         <v>39</v>
       </c>
       <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
         <v>3</v>
       </c>
     </row>

</xml_diff>